<commit_message>
Until Part 2 Chapter 14
</commit_message>
<xml_diff>
--- a/P2C12/txtToExcel.xlsx
+++ b/P2C12/txtToExcel.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,7 +14,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">5. C
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. B
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. D
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. D
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. D
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. C
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. A
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. A
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. B
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. D
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. B
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. A
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. B
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. A
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. C
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. D
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. C
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. C
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. B
+</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -348,14 +429,865 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>